<commit_message>
Done Done! Made final changes.
</commit_message>
<xml_diff>
--- a/Bardewa_OConnell/code/Verification/resultVerification.xlsx
+++ b/Bardewa_OConnell/code/Verification/resultVerification.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="6">
   <si>
     <t>Expected</t>
   </si>
@@ -29,6 +29,15 @@
   </si>
   <si>
     <t>Processor Out</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>o</t>
   </si>
 </sst>
 </file>
@@ -393,7 +402,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -415,31 +424,55 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
       <c r="C2" t="b">
         <f>A2=B2</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" s="2" t="b">
         <f>List1=List2</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
       <c r="C3" t="b">
         <f t="shared" ref="C3:C5" si="0">A3=B3</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
       <c r="C4" t="b">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
       <c r="C5" t="b">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>